<commit_message>
WM part of doku ready to be submitted
</commit_message>
<xml_diff>
--- a/SchnippSchnapp GmbH.xlsx
+++ b/SchnippSchnapp GmbH.xlsx
@@ -1,21 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandra .DESKTOP-P6HT5MR\Desktop\4.Semester\SAP Modellierung\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF2EFB6-2826-4F03-A38F-089B560467A7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16560" windowHeight="11640" xr2:uid="{636DFFD2-404C-415A-8852-740D2A6B8B9D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16560" windowHeight="11640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelle4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="68">
   <si>
     <t>SchnippSchnapp GmbH</t>
   </si>
@@ -211,16 +208,34 @@
   </si>
   <si>
     <t xml:space="preserve">1x Verschlussöffner </t>
+  </si>
+  <si>
+    <t>TR-CM</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>Woche</t>
+  </si>
+  <si>
+    <t>Kosten pro Person pro Tag</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>Kosten insgesamt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +246,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -286,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -674,11 +697,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -748,6 +839,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1054,39 +1182,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77F1B4B-5415-4DD3-BC96-F4076FA3778F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="C72" sqref="C72"/>
+      <selection pane="topRight" activeCell="X56" sqref="X56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1328125" customWidth="1"/>
-    <col min="2" max="2" width="16.46484375" customWidth="1"/>
-    <col min="3" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" customWidth="1"/>
-    <col min="9" max="9" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.6640625" customWidth="1"/>
-    <col min="28" max="28" width="10.53125" customWidth="1"/>
-    <col min="29" max="29" width="10.86328125" customWidth="1"/>
-    <col min="30" max="30" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" customWidth="1"/>
+    <col min="28" max="28" width="10.5703125" customWidth="1"/>
+    <col min="29" max="29" width="10.85546875" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1135,7 +1263,7 @@
       <c r="J2" s="37"/>
       <c r="K2" s="16"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
@@ -1158,7 +1286,7 @@
       </c>
       <c r="K3" s="16"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="28" t="s">
         <v>2</v>
       </c>
@@ -1177,7 +1305,7 @@
       <c r="J4" s="28"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="28" t="s">
         <v>3</v>
       </c>
@@ -1196,7 +1324,7 @@
       <c r="J5" s="28"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="28" t="s">
         <v>4</v>
       </c>
@@ -1215,7 +1343,7 @@
       <c r="J6" s="28"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="28" t="s">
         <v>5</v>
       </c>
@@ -1236,7 +1364,7 @@
       <c r="J7" s="28"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="28" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1397,7 @@
       </c>
       <c r="K8" s="16"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="28" t="s">
         <v>7</v>
       </c>
@@ -1286,7 +1414,7 @@
       <c r="J9" s="28"/>
       <c r="K9" s="16"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="28" t="s">
         <v>8</v>
       </c>
@@ -1303,7 +1431,7 @@
       <c r="J10" s="28"/>
       <c r="K10" s="16"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
         <v>9</v>
       </c>
@@ -1336,7 +1464,7 @@
       </c>
       <c r="K11" s="16"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="28" t="s">
         <v>10</v>
       </c>
@@ -1414,7 +1542,7 @@
       </c>
       <c r="K14" s="16"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="34" t="s">
         <v>22</v>
       </c>
@@ -1445,7 +1573,7 @@
       </c>
       <c r="K15" s="16"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="34" t="s">
         <v>24</v>
       </c>
@@ -1514,7 +1642,7 @@
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:47" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1527,7 +1655,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="22" spans="1:47" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:47" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="22"/>
       <c r="B22" s="45">
         <v>1</v>
@@ -1668,7 +1796,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:47" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
         <v>1</v>
       </c>
@@ -1727,7 +1855,7 @@
       <c r="AT23" s="15"/>
       <c r="AU23" s="15"/>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
         <v>2</v>
       </c>
@@ -1778,7 +1906,7 @@
       <c r="AT24" s="21"/>
       <c r="AU24" s="21"/>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>3</v>
       </c>
@@ -1829,7 +1957,7 @@
       <c r="AT25" s="21"/>
       <c r="AU25" s="21"/>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>4</v>
       </c>
@@ -1880,7 +2008,7 @@
       <c r="AT26" s="21"/>
       <c r="AU26" s="21"/>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
         <v>5</v>
       </c>
@@ -1931,7 +2059,7 @@
       <c r="AT27" s="21"/>
       <c r="AU27" s="21"/>
     </row>
-    <row r="28" spans="1:47" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="49" t="s">
         <v>6</v>
       </c>
@@ -2309,7 +2437,7 @@
       <c r="AT33" s="53"/>
       <c r="AU33" s="58"/>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:47" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="50" t="s">
         <v>36</v>
       </c>
@@ -2405,7 +2533,7 @@
       <c r="AT34" s="57"/>
       <c r="AU34" s="39"/>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:47" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="50" t="s">
         <v>33</v>
       </c>
@@ -2471,7 +2599,7 @@
       <c r="AT35" s="57"/>
       <c r="AU35" s="39"/>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:47" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="50" t="s">
         <v>34</v>
       </c>
@@ -2786,7 +2914,7 @@
         <v>97000</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:47" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B40" s="5" t="s">
         <v>32</v>
       </c>
@@ -2806,7 +2934,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:47" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
         <v>43</v>
       </c>
@@ -2835,7 +2963,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:47" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G42" t="s">
         <v>46</v>
       </c>
@@ -2846,7 +2974,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:47" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B47" s="7" t="s">
         <v>27</v>
       </c>
@@ -2863,7 +2991,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:47" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G48" t="s">
         <v>43</v>
       </c>
@@ -2883,7 +3011,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G49" t="s">
         <v>46</v>
       </c>
@@ -2903,12 +3031,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
         <v>41</v>
       </c>
@@ -2919,7 +3047,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B53" t="s">
         <v>43</v>
       </c>
@@ -2943,7 +3071,7 @@
         <v>1550000</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G54" t="s">
         <v>46</v>
       </c>
@@ -2954,12 +3082,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
         <v>44</v>
       </c>
@@ -2973,7 +3101,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G57" t="s">
         <v>46</v>
       </c>
@@ -2984,7 +3112,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>50</v>
       </c>
@@ -2992,7 +3120,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>58</v>
       </c>
@@ -3000,7 +3128,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
         <v>51</v>
       </c>
@@ -3008,32 +3136,32 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:2" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:2" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>61</v>
       </c>
@@ -3048,4 +3176,2410 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="37"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="29">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="29">
+        <v>365</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="28"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="29">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="28"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="29">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="28"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="29">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>10</v>
+      </c>
+      <c r="J7" s="28"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="29">
+        <v>40</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="29">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="29">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="28"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="29">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="29">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="28"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="31">
+        <v>5</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26">
+        <v>5</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="36"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="33">
+        <f>SUM(B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13)</f>
+        <v>505</v>
+      </c>
+      <c r="C14" s="27">
+        <f>SUM(C2:C13)</f>
+        <v>6</v>
+      </c>
+      <c r="D14" s="27">
+        <f t="shared" ref="D14:J14" si="0">SUM(D2:D13)</f>
+        <v>7</v>
+      </c>
+      <c r="E14" s="27">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F14" s="27">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G14" s="27">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="H14" s="27">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="I14" s="27">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J14" s="37">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="4">
+        <v>417</v>
+      </c>
+      <c r="D15" s="4">
+        <v>250</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3750</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4000</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2500</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1500</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2000</v>
+      </c>
+      <c r="J15" s="38">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="35"/>
+      <c r="C16" s="4">
+        <f>C14*C15</f>
+        <v>2502</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" ref="D16:F16" si="1">D14*D15</f>
+        <v>1750</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>11250</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>68000</v>
+      </c>
+      <c r="G16" s="4">
+        <f>G14*G15</f>
+        <v>55000</v>
+      </c>
+      <c r="H16" s="4">
+        <f>H14*H15</f>
+        <v>31500</v>
+      </c>
+      <c r="I16" s="4">
+        <f>I14*I15</f>
+        <v>24000</v>
+      </c>
+      <c r="J16" s="38">
+        <f>J14*J15</f>
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="40">
+        <f>SUM(C16:J16)</f>
+        <v>198202</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="42"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A21:AU66"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A9" sqref="A9"/>
+      <selection pane="topRight" activeCell="K56" sqref="K56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="21" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:47" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="45">
+        <v>1</v>
+      </c>
+      <c r="C22" s="44">
+        <v>2</v>
+      </c>
+      <c r="D22" s="44">
+        <v>3</v>
+      </c>
+      <c r="E22" s="44">
+        <v>4</v>
+      </c>
+      <c r="F22" s="44">
+        <v>5</v>
+      </c>
+      <c r="G22" s="44">
+        <v>6</v>
+      </c>
+      <c r="H22" s="44">
+        <v>7</v>
+      </c>
+      <c r="I22" s="44">
+        <v>8</v>
+      </c>
+      <c r="J22" s="44">
+        <v>9</v>
+      </c>
+      <c r="K22" s="44">
+        <v>10</v>
+      </c>
+      <c r="L22" s="44">
+        <v>11</v>
+      </c>
+      <c r="M22" s="44">
+        <v>12</v>
+      </c>
+      <c r="N22" s="44">
+        <v>13</v>
+      </c>
+      <c r="O22" s="44">
+        <v>14</v>
+      </c>
+      <c r="P22" s="44">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="44">
+        <v>16</v>
+      </c>
+      <c r="R22" s="44">
+        <v>17</v>
+      </c>
+      <c r="S22" s="44">
+        <v>18</v>
+      </c>
+      <c r="T22" s="44">
+        <v>19</v>
+      </c>
+      <c r="U22" s="44">
+        <v>20</v>
+      </c>
+      <c r="V22" s="44">
+        <v>21</v>
+      </c>
+      <c r="W22" s="44">
+        <v>22</v>
+      </c>
+      <c r="X22" s="44">
+        <v>23</v>
+      </c>
+      <c r="Y22" s="44">
+        <v>24</v>
+      </c>
+      <c r="Z22" s="44">
+        <v>25</v>
+      </c>
+      <c r="AA22" s="44">
+        <v>26</v>
+      </c>
+      <c r="AB22" s="44">
+        <v>27</v>
+      </c>
+      <c r="AC22" s="44">
+        <v>28</v>
+      </c>
+      <c r="AD22" s="44">
+        <v>29</v>
+      </c>
+      <c r="AE22" s="46">
+        <v>30</v>
+      </c>
+      <c r="AF22" s="44">
+        <v>31</v>
+      </c>
+      <c r="AG22" s="46">
+        <v>32</v>
+      </c>
+      <c r="AH22" s="44">
+        <v>33</v>
+      </c>
+      <c r="AI22" s="46">
+        <v>34</v>
+      </c>
+      <c r="AJ22" s="44">
+        <v>35</v>
+      </c>
+      <c r="AK22" s="46">
+        <v>36</v>
+      </c>
+      <c r="AL22" s="44">
+        <v>37</v>
+      </c>
+      <c r="AM22" s="46">
+        <v>38</v>
+      </c>
+      <c r="AN22" s="44">
+        <v>39</v>
+      </c>
+      <c r="AO22" s="46">
+        <v>40</v>
+      </c>
+      <c r="AP22" s="44">
+        <v>41</v>
+      </c>
+      <c r="AQ22" s="46">
+        <v>42</v>
+      </c>
+      <c r="AR22" s="44">
+        <v>43</v>
+      </c>
+      <c r="AS22" s="46">
+        <v>44</v>
+      </c>
+      <c r="AT22" s="44">
+        <v>45</v>
+      </c>
+      <c r="AU22" s="46">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="O23" s="60"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="14"/>
+      <c r="AD23" s="14"/>
+      <c r="AE23" s="14"/>
+      <c r="AF23" s="14"/>
+      <c r="AG23" s="14"/>
+      <c r="AH23" s="14"/>
+      <c r="AI23" s="14"/>
+      <c r="AJ23" s="14"/>
+      <c r="AK23" s="14"/>
+      <c r="AL23" s="14"/>
+      <c r="AM23" s="14"/>
+      <c r="AN23" s="14"/>
+      <c r="AO23" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP23" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ23" s="60"/>
+      <c r="AR23" s="60"/>
+      <c r="AS23" s="60"/>
+      <c r="AT23" s="15"/>
+      <c r="AU23" s="63"/>
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="18"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="17"/>
+      <c r="AA24" s="17"/>
+      <c r="AB24" s="17"/>
+      <c r="AC24" s="17"/>
+      <c r="AD24" s="17"/>
+      <c r="AE24" s="17"/>
+      <c r="AF24" s="17"/>
+      <c r="AG24" s="17"/>
+      <c r="AH24" s="17"/>
+      <c r="AI24" s="17"/>
+      <c r="AJ24" s="17"/>
+      <c r="AK24" s="17"/>
+      <c r="AL24" s="17"/>
+      <c r="AM24" s="17"/>
+      <c r="AN24" s="17"/>
+      <c r="AO24" s="75"/>
+      <c r="AP24" s="61"/>
+      <c r="AQ24" s="61"/>
+      <c r="AR24" s="61"/>
+      <c r="AS24" s="61"/>
+      <c r="AT24" s="21"/>
+      <c r="AU24" s="64"/>
+    </row>
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A25" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="61"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="18"/>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="19"/>
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="20"/>
+      <c r="AC25" s="17"/>
+      <c r="AD25" s="17"/>
+      <c r="AE25" s="17"/>
+      <c r="AF25" s="17"/>
+      <c r="AG25" s="17"/>
+      <c r="AH25" s="17"/>
+      <c r="AI25" s="17"/>
+      <c r="AJ25" s="17"/>
+      <c r="AK25" s="17"/>
+      <c r="AL25" s="17"/>
+      <c r="AM25" s="17"/>
+      <c r="AN25" s="17"/>
+      <c r="AO25" s="75"/>
+      <c r="AP25" s="61"/>
+      <c r="AQ25" s="61"/>
+      <c r="AR25" s="61"/>
+      <c r="AS25" s="61"/>
+      <c r="AT25" s="21"/>
+      <c r="AU25" s="64"/>
+    </row>
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A26" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="61"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+      <c r="Z26" s="17"/>
+      <c r="AA26" s="17"/>
+      <c r="AB26" s="18"/>
+      <c r="AC26" s="19"/>
+      <c r="AD26" s="19"/>
+      <c r="AE26" s="19"/>
+      <c r="AF26" s="20"/>
+      <c r="AG26" s="17"/>
+      <c r="AH26" s="17"/>
+      <c r="AI26" s="17"/>
+      <c r="AJ26" s="17"/>
+      <c r="AK26" s="17"/>
+      <c r="AL26" s="17"/>
+      <c r="AM26" s="17"/>
+      <c r="AN26" s="17"/>
+      <c r="AO26" s="75"/>
+      <c r="AP26" s="61"/>
+      <c r="AQ26" s="61"/>
+      <c r="AR26" s="61"/>
+      <c r="AS26" s="61"/>
+      <c r="AT26" s="21"/>
+      <c r="AU26" s="64"/>
+    </row>
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A27" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="17"/>
+      <c r="Z27" s="17"/>
+      <c r="AA27" s="17"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="17"/>
+      <c r="AD27" s="17"/>
+      <c r="AE27" s="17"/>
+      <c r="AF27" s="18"/>
+      <c r="AG27" s="19"/>
+      <c r="AH27" s="19"/>
+      <c r="AI27" s="19"/>
+      <c r="AJ27" s="20"/>
+      <c r="AK27" s="17"/>
+      <c r="AL27" s="17"/>
+      <c r="AM27" s="17"/>
+      <c r="AN27" s="17"/>
+      <c r="AO27" s="75"/>
+      <c r="AP27" s="61"/>
+      <c r="AQ27" s="61"/>
+      <c r="AR27" s="61"/>
+      <c r="AS27" s="61"/>
+      <c r="AT27" s="21"/>
+      <c r="AU27" s="64"/>
+    </row>
+    <row r="28" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="24"/>
+      <c r="U28" s="24"/>
+      <c r="V28" s="24"/>
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="24"/>
+      <c r="Z28" s="24"/>
+      <c r="AA28" s="24"/>
+      <c r="AB28" s="24"/>
+      <c r="AC28" s="24"/>
+      <c r="AD28" s="24"/>
+      <c r="AE28" s="24"/>
+      <c r="AF28" s="24"/>
+      <c r="AG28" s="24"/>
+      <c r="AH28" s="24"/>
+      <c r="AI28" s="24"/>
+      <c r="AJ28" s="55"/>
+      <c r="AK28" s="56"/>
+      <c r="AL28" s="56"/>
+      <c r="AM28" s="56"/>
+      <c r="AN28" s="56"/>
+      <c r="AO28" s="76"/>
+      <c r="AP28" s="62"/>
+      <c r="AQ28" s="62"/>
+      <c r="AR28" s="62"/>
+      <c r="AS28" s="62"/>
+      <c r="AT28" s="25"/>
+      <c r="AU28" s="65"/>
+    </row>
+    <row r="29" spans="1:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="C29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="D29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="E29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="F29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="G29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="H29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="I29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="J29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="K29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="L29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="M29" s="53">
+        <f>5*$C$52*$D$52</f>
+        <v>48000</v>
+      </c>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
+      <c r="S29" s="53"/>
+      <c r="T29" s="53"/>
+      <c r="U29" s="53"/>
+      <c r="V29" s="53"/>
+      <c r="W29" s="53"/>
+      <c r="X29" s="53"/>
+      <c r="Y29" s="53"/>
+      <c r="Z29" s="53"/>
+      <c r="AA29" s="53"/>
+      <c r="AB29" s="53"/>
+      <c r="AC29" s="53"/>
+      <c r="AD29" s="53"/>
+      <c r="AE29" s="53"/>
+      <c r="AF29" s="53"/>
+      <c r="AG29" s="53"/>
+      <c r="AH29" s="53"/>
+      <c r="AI29" s="53"/>
+      <c r="AJ29" s="53"/>
+      <c r="AK29" s="53"/>
+      <c r="AL29" s="53"/>
+      <c r="AM29" s="53"/>
+      <c r="AN29" s="53"/>
+      <c r="AO29" s="53"/>
+      <c r="AP29" s="53"/>
+      <c r="AQ29" s="53"/>
+      <c r="AR29" s="53"/>
+      <c r="AS29" s="53"/>
+      <c r="AT29" s="53"/>
+      <c r="AU29" s="58"/>
+    </row>
+    <row r="30" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="54">
+        <f>5*$C$55*$D$55</f>
+        <v>8000</v>
+      </c>
+      <c r="O30" s="54">
+        <f>5*$C$55*$D$55</f>
+        <v>8000</v>
+      </c>
+      <c r="P30" s="54"/>
+      <c r="Q30" s="54"/>
+      <c r="R30" s="54"/>
+      <c r="S30" s="54"/>
+      <c r="T30" s="54"/>
+      <c r="U30" s="54"/>
+      <c r="V30" s="54"/>
+      <c r="W30" s="54"/>
+      <c r="X30" s="54"/>
+      <c r="Y30" s="54"/>
+      <c r="Z30" s="54"/>
+      <c r="AA30" s="54"/>
+      <c r="AB30" s="54"/>
+      <c r="AC30" s="54"/>
+      <c r="AD30" s="54"/>
+      <c r="AE30" s="54"/>
+      <c r="AF30" s="54"/>
+      <c r="AG30" s="54"/>
+      <c r="AH30" s="54"/>
+      <c r="AI30" s="54"/>
+      <c r="AJ30" s="54"/>
+      <c r="AK30" s="54"/>
+      <c r="AL30" s="54"/>
+      <c r="AM30" s="54"/>
+      <c r="AN30" s="54"/>
+      <c r="AO30" s="54"/>
+      <c r="AP30" s="54"/>
+      <c r="AQ30" s="54"/>
+      <c r="AR30" s="54"/>
+      <c r="AS30" s="54"/>
+      <c r="AT30" s="54"/>
+      <c r="AU30" s="59"/>
+    </row>
+    <row r="31" spans="1:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="57"/>
+      <c r="Q31" s="57"/>
+      <c r="R31" s="57"/>
+      <c r="S31" s="57"/>
+      <c r="T31" s="57"/>
+      <c r="U31" s="57"/>
+      <c r="V31" s="57"/>
+      <c r="W31" s="57"/>
+      <c r="X31" s="57"/>
+      <c r="Y31" s="57"/>
+      <c r="Z31" s="57"/>
+      <c r="AA31" s="57"/>
+      <c r="AB31" s="57"/>
+      <c r="AC31" s="57"/>
+      <c r="AD31" s="57"/>
+      <c r="AE31" s="57"/>
+      <c r="AF31" s="57"/>
+      <c r="AG31" s="57"/>
+      <c r="AH31" s="57"/>
+      <c r="AI31" s="57"/>
+      <c r="AJ31" s="57"/>
+      <c r="AK31" s="57"/>
+      <c r="AL31" s="57"/>
+      <c r="AM31" s="57"/>
+      <c r="AN31" s="57"/>
+      <c r="AO31" s="57">
+        <f>5*$H$53*$I$53+5*$H$54*$I$54</f>
+        <v>16000</v>
+      </c>
+      <c r="AP31" s="57"/>
+      <c r="AQ31" s="57"/>
+      <c r="AR31" s="57"/>
+      <c r="AS31" s="57"/>
+      <c r="AT31" s="57"/>
+      <c r="AU31" s="39"/>
+    </row>
+    <row r="32" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="57"/>
+      <c r="L32" s="57"/>
+      <c r="M32" s="57"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="57"/>
+      <c r="P32" s="57"/>
+      <c r="Q32" s="57"/>
+      <c r="R32" s="57"/>
+      <c r="S32" s="57"/>
+      <c r="T32" s="57"/>
+      <c r="U32" s="57"/>
+      <c r="V32" s="57"/>
+      <c r="W32" s="57"/>
+      <c r="X32" s="57"/>
+      <c r="Y32" s="57"/>
+      <c r="Z32" s="57"/>
+      <c r="AA32" s="57"/>
+      <c r="AB32" s="57"/>
+      <c r="AC32" s="57"/>
+      <c r="AD32" s="57"/>
+      <c r="AE32" s="57"/>
+      <c r="AF32" s="57"/>
+      <c r="AG32" s="57"/>
+      <c r="AH32" s="57"/>
+      <c r="AI32" s="57"/>
+      <c r="AJ32" s="57"/>
+      <c r="AK32" s="57"/>
+      <c r="AL32" s="57"/>
+      <c r="AM32" s="57"/>
+      <c r="AN32" s="57"/>
+      <c r="AO32" s="57"/>
+      <c r="AP32" s="57">
+        <f>5*$H$57*$I$57</f>
+        <v>20000</v>
+      </c>
+      <c r="AQ32" s="57">
+        <f t="shared" ref="AQ32:AS32" si="0">5*$H$57*$I$57</f>
+        <v>20000</v>
+      </c>
+      <c r="AR32" s="57">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="AS32" s="57">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="AT32" s="57"/>
+      <c r="AU32" s="39"/>
+    </row>
+    <row r="33" spans="1:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="53"/>
+      <c r="N33" s="53"/>
+      <c r="O33" s="53"/>
+      <c r="P33" s="53">
+        <f>5*$C$41*$D$41</f>
+        <v>12000</v>
+      </c>
+      <c r="Q33" s="53"/>
+      <c r="R33" s="53"/>
+      <c r="S33" s="53"/>
+      <c r="T33" s="53">
+        <f>5*$C$41*$D$41</f>
+        <v>12000</v>
+      </c>
+      <c r="U33" s="53"/>
+      <c r="V33" s="53"/>
+      <c r="W33" s="53"/>
+      <c r="X33" s="53">
+        <f>5*$C$41*$D$41</f>
+        <v>12000</v>
+      </c>
+      <c r="Y33" s="53"/>
+      <c r="Z33" s="53"/>
+      <c r="AA33" s="53"/>
+      <c r="AB33" s="53">
+        <f>5*$C$41*$D$41</f>
+        <v>12000</v>
+      </c>
+      <c r="AC33" s="53"/>
+      <c r="AD33" s="53"/>
+      <c r="AE33" s="53"/>
+      <c r="AF33" s="53">
+        <f>5*$C$41*$D$41</f>
+        <v>12000</v>
+      </c>
+      <c r="AG33" s="53"/>
+      <c r="AH33" s="53"/>
+      <c r="AI33" s="53"/>
+      <c r="AJ33" s="53"/>
+      <c r="AK33" s="53"/>
+      <c r="AL33" s="53"/>
+      <c r="AM33" s="53"/>
+      <c r="AN33" s="53"/>
+      <c r="AO33" s="53"/>
+      <c r="AP33" s="53"/>
+      <c r="AQ33" s="53"/>
+      <c r="AR33" s="53"/>
+      <c r="AS33" s="53"/>
+      <c r="AT33" s="53"/>
+      <c r="AU33" s="58"/>
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A34" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="57"/>
+      <c r="M34" s="57"/>
+      <c r="N34" s="57"/>
+      <c r="O34" s="57"/>
+      <c r="P34" s="57"/>
+      <c r="Q34" s="57">
+        <f>5*$H$41*$I$41+5*$H$42*$I$42</f>
+        <v>32000</v>
+      </c>
+      <c r="R34" s="57">
+        <f t="shared" ref="R34:S34" si="1">5*$H$41*$I$41+5*$H$42*$I$42</f>
+        <v>32000</v>
+      </c>
+      <c r="S34" s="57">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="T34" s="57"/>
+      <c r="U34" s="57">
+        <f>5*$H$41*$I$41+5*$H$42*$I$42</f>
+        <v>32000</v>
+      </c>
+      <c r="V34" s="57">
+        <f t="shared" ref="V34:W34" si="2">5*$H$41*$I$41+5*$H$42*$I$42</f>
+        <v>32000</v>
+      </c>
+      <c r="W34" s="57">
+        <f t="shared" si="2"/>
+        <v>32000</v>
+      </c>
+      <c r="X34" s="57"/>
+      <c r="Y34" s="57">
+        <f>5*$H$41*$I$41+5*$H$42*$I$42</f>
+        <v>32000</v>
+      </c>
+      <c r="Z34" s="57">
+        <f t="shared" ref="Z34:AA34" si="3">5*$H$41*$I$41+5*$H$42*$I$42</f>
+        <v>32000</v>
+      </c>
+      <c r="AA34" s="57">
+        <f t="shared" si="3"/>
+        <v>32000</v>
+      </c>
+      <c r="AB34" s="57"/>
+      <c r="AC34" s="57">
+        <f>5*$H$41*$I$41+5*$H$42*$I$42</f>
+        <v>32000</v>
+      </c>
+      <c r="AD34" s="57">
+        <f t="shared" ref="AD34:AE34" si="4">5*$H$41*$I$41+5*$H$42*$I$42</f>
+        <v>32000</v>
+      </c>
+      <c r="AE34" s="57">
+        <f t="shared" si="4"/>
+        <v>32000</v>
+      </c>
+      <c r="AF34" s="57"/>
+      <c r="AG34" s="57">
+        <f>5*$H$41*$I$41+5*$H$42*$I$42</f>
+        <v>32000</v>
+      </c>
+      <c r="AH34" s="57">
+        <f t="shared" ref="AH34:AI34" si="5">5*$H$41*$I$41+5*$H$42*$I$42</f>
+        <v>32000</v>
+      </c>
+      <c r="AI34" s="57">
+        <f t="shared" si="5"/>
+        <v>32000</v>
+      </c>
+      <c r="AJ34" s="57"/>
+      <c r="AK34" s="57"/>
+      <c r="AL34" s="57"/>
+      <c r="AM34" s="57"/>
+      <c r="AN34" s="57"/>
+      <c r="AO34" s="57"/>
+      <c r="AP34" s="57"/>
+      <c r="AQ34" s="57"/>
+      <c r="AR34" s="57"/>
+      <c r="AS34" s="57"/>
+      <c r="AT34" s="57"/>
+      <c r="AU34" s="39"/>
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A35" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="57"/>
+      <c r="M35" s="57"/>
+      <c r="N35" s="57"/>
+      <c r="O35" s="57"/>
+      <c r="P35" s="57"/>
+      <c r="Q35" s="57"/>
+      <c r="R35" s="57"/>
+      <c r="S35" s="57"/>
+      <c r="T35" s="57">
+        <f>5*$H$48*$I$48+5*$H$49*$I$49</f>
+        <v>16000</v>
+      </c>
+      <c r="U35" s="57"/>
+      <c r="V35" s="57"/>
+      <c r="W35" s="57"/>
+      <c r="X35" s="57">
+        <f>5*$H$48*$I$48+5*$H$49*$I$49</f>
+        <v>16000</v>
+      </c>
+      <c r="Y35" s="57"/>
+      <c r="Z35" s="57"/>
+      <c r="AA35" s="57"/>
+      <c r="AB35" s="57">
+        <f>5*$H$48*$I$48+5*$H$49*$I$49</f>
+        <v>16000</v>
+      </c>
+      <c r="AC35" s="57"/>
+      <c r="AD35" s="57"/>
+      <c r="AE35" s="57"/>
+      <c r="AF35" s="57">
+        <f>5*$H$48*$I$48+5*$H$49*$I$49</f>
+        <v>16000</v>
+      </c>
+      <c r="AG35" s="57"/>
+      <c r="AH35" s="57"/>
+      <c r="AI35" s="57"/>
+      <c r="AJ35" s="57">
+        <f>5*$H$48*$I$48+5*$H$49*$I$49</f>
+        <v>16000</v>
+      </c>
+      <c r="AK35" s="57"/>
+      <c r="AL35" s="57"/>
+      <c r="AM35" s="57"/>
+      <c r="AN35" s="57"/>
+      <c r="AO35" s="57"/>
+      <c r="AP35" s="57"/>
+      <c r="AQ35" s="57"/>
+      <c r="AR35" s="57"/>
+      <c r="AS35" s="57"/>
+      <c r="AT35" s="57"/>
+      <c r="AU35" s="39"/>
+    </row>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A36" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="57"/>
+      <c r="M36" s="57"/>
+      <c r="N36" s="57"/>
+      <c r="O36" s="57"/>
+      <c r="P36" s="57"/>
+      <c r="Q36" s="57"/>
+      <c r="R36" s="57"/>
+      <c r="S36" s="57"/>
+      <c r="T36" s="57"/>
+      <c r="U36" s="57"/>
+      <c r="V36" s="57"/>
+      <c r="W36" s="57"/>
+      <c r="X36" s="57"/>
+      <c r="Y36" s="57"/>
+      <c r="Z36" s="57"/>
+      <c r="AA36" s="57"/>
+      <c r="AB36" s="57"/>
+      <c r="AC36" s="57"/>
+      <c r="AD36" s="57"/>
+      <c r="AE36" s="57"/>
+      <c r="AF36" s="57"/>
+      <c r="AG36" s="57"/>
+      <c r="AH36" s="57"/>
+      <c r="AI36" s="57"/>
+      <c r="AJ36" s="57"/>
+      <c r="AK36" s="57"/>
+      <c r="AL36" s="57"/>
+      <c r="AM36" s="57"/>
+      <c r="AN36" s="57"/>
+      <c r="AO36" s="57"/>
+      <c r="AP36" s="57"/>
+      <c r="AQ36" s="57"/>
+      <c r="AR36" s="57"/>
+      <c r="AS36" s="57"/>
+      <c r="AT36" s="57">
+        <f>5*$N$49*$O$49</f>
+        <v>25000</v>
+      </c>
+      <c r="AU36" s="39">
+        <f>5*$N$49*$O$49</f>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="54"/>
+      <c r="L37" s="54"/>
+      <c r="M37" s="54"/>
+      <c r="N37" s="54"/>
+      <c r="O37" s="54"/>
+      <c r="P37" s="54"/>
+      <c r="Q37" s="54"/>
+      <c r="R37" s="54"/>
+      <c r="S37" s="54"/>
+      <c r="T37" s="54"/>
+      <c r="U37" s="54"/>
+      <c r="V37" s="54"/>
+      <c r="W37" s="54"/>
+      <c r="X37" s="54"/>
+      <c r="Y37" s="54"/>
+      <c r="Z37" s="54"/>
+      <c r="AA37" s="54"/>
+      <c r="AB37" s="54"/>
+      <c r="AC37" s="54"/>
+      <c r="AD37" s="54"/>
+      <c r="AE37" s="54"/>
+      <c r="AF37" s="54"/>
+      <c r="AG37" s="54"/>
+      <c r="AH37" s="54"/>
+      <c r="AI37" s="54"/>
+      <c r="AJ37" s="54"/>
+      <c r="AK37" s="54">
+        <f>5*$N$41*$O$41</f>
+        <v>12000</v>
+      </c>
+      <c r="AL37" s="54">
+        <f t="shared" ref="AL37:AN37" si="6">5*$N$41*$O$41</f>
+        <v>12000</v>
+      </c>
+      <c r="AM37" s="54">
+        <f t="shared" si="6"/>
+        <v>12000</v>
+      </c>
+      <c r="AN37" s="54">
+        <f t="shared" si="6"/>
+        <v>12000</v>
+      </c>
+      <c r="AO37" s="54"/>
+      <c r="AP37" s="54"/>
+      <c r="AQ37" s="54"/>
+      <c r="AR37" s="54"/>
+      <c r="AS37" s="54"/>
+      <c r="AT37" s="54">
+        <f>5*$N$48*$O$48</f>
+        <v>72000</v>
+      </c>
+      <c r="AU37" s="59">
+        <f>5*$N$48*$O$48</f>
+        <v>72000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="57">
+        <f>SUM(B29:B37)</f>
+        <v>48000</v>
+      </c>
+      <c r="C38" s="57">
+        <f t="shared" ref="C38:AU38" si="7">SUM(C29:C37)</f>
+        <v>48000</v>
+      </c>
+      <c r="D38" s="57">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="E38" s="57">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="F38" s="57">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="G38" s="57">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="H38" s="57">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="I38" s="57">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="J38" s="57">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="K38" s="57">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="L38" s="57">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="M38" s="57">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="N38" s="57">
+        <f t="shared" si="7"/>
+        <v>8000</v>
+      </c>
+      <c r="O38" s="57">
+        <f t="shared" si="7"/>
+        <v>8000</v>
+      </c>
+      <c r="P38" s="57">
+        <f t="shared" si="7"/>
+        <v>12000</v>
+      </c>
+      <c r="Q38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="R38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="S38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="T38" s="57">
+        <f t="shared" si="7"/>
+        <v>28000</v>
+      </c>
+      <c r="U38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="V38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="W38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="X38" s="57">
+        <f t="shared" si="7"/>
+        <v>28000</v>
+      </c>
+      <c r="Y38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="Z38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="AA38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="AB38" s="57">
+        <f t="shared" si="7"/>
+        <v>28000</v>
+      </c>
+      <c r="AC38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="AD38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="AE38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="AF38" s="57">
+        <f t="shared" si="7"/>
+        <v>28000</v>
+      </c>
+      <c r="AG38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="AH38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="AI38" s="57">
+        <f t="shared" si="7"/>
+        <v>32000</v>
+      </c>
+      <c r="AJ38" s="57">
+        <f t="shared" si="7"/>
+        <v>16000</v>
+      </c>
+      <c r="AK38" s="57">
+        <f t="shared" si="7"/>
+        <v>12000</v>
+      </c>
+      <c r="AL38" s="57">
+        <f t="shared" si="7"/>
+        <v>12000</v>
+      </c>
+      <c r="AM38" s="57">
+        <f t="shared" si="7"/>
+        <v>12000</v>
+      </c>
+      <c r="AN38" s="57">
+        <f t="shared" si="7"/>
+        <v>12000</v>
+      </c>
+      <c r="AO38" s="57">
+        <f t="shared" si="7"/>
+        <v>16000</v>
+      </c>
+      <c r="AP38" s="57">
+        <f t="shared" si="7"/>
+        <v>20000</v>
+      </c>
+      <c r="AQ38" s="57">
+        <f t="shared" si="7"/>
+        <v>20000</v>
+      </c>
+      <c r="AR38" s="57">
+        <f t="shared" si="7"/>
+        <v>20000</v>
+      </c>
+      <c r="AS38" s="57">
+        <f t="shared" si="7"/>
+        <v>20000</v>
+      </c>
+      <c r="AT38" s="57">
+        <f t="shared" si="7"/>
+        <v>97000</v>
+      </c>
+      <c r="AU38" s="57">
+        <f t="shared" si="7"/>
+        <v>97000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" t="s">
+        <v>45</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" t="s">
+        <v>45</v>
+      </c>
+      <c r="M40" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>1200</v>
+      </c>
+      <c r="G41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>1200</v>
+      </c>
+      <c r="M41" t="s">
+        <v>43</v>
+      </c>
+      <c r="N41">
+        <v>2</v>
+      </c>
+      <c r="O41">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="G47" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I47" t="s">
+        <v>45</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M47" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="N47" s="69"/>
+      <c r="O47" s="69"/>
+      <c r="S47" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="T47" s="69"/>
+      <c r="U47" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="V47" s="69"/>
+      <c r="W47" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="X47" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y47" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z47" s="69"/>
+      <c r="AA47" s="69"/>
+    </row>
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>1200</v>
+      </c>
+      <c r="M48" t="s">
+        <v>43</v>
+      </c>
+      <c r="N48">
+        <v>12</v>
+      </c>
+      <c r="O48">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>46</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>1000</v>
+      </c>
+      <c r="M49" t="s">
+        <v>46</v>
+      </c>
+      <c r="N49">
+        <v>5</v>
+      </c>
+      <c r="O49">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52">
+        <v>8</v>
+      </c>
+      <c r="D52">
+        <v>1200</v>
+      </c>
+      <c r="G52" t="s">
+        <v>47</v>
+      </c>
+      <c r="M52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>43</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>1200</v>
+      </c>
+      <c r="M53" s="66">
+        <f>SUM(B38:AU38)</f>
+        <v>1550000</v>
+      </c>
+      <c r="N53" s="67"/>
+      <c r="O53" s="67"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>38</v>
+      </c>
+      <c r="G54" t="s">
+        <v>46</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>46</v>
+      </c>
+      <c r="H57">
+        <v>4</v>
+      </c>
+      <c r="I57">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B23:M28"/>
+    <mergeCell ref="N23:O28"/>
+    <mergeCell ref="AO23:AO28"/>
+    <mergeCell ref="AP23:AS28"/>
+    <mergeCell ref="M53:O53"/>
+    <mergeCell ref="M47:O47"/>
+    <mergeCell ref="Y47:AA47"/>
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="U47:V47"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>1200</v>
+      </c>
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1200</v>
+      </c>
+      <c r="M10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10">
+        <v>12</v>
+      </c>
+      <c r="O10">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>1000</v>
+      </c>
+      <c r="M11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="77"/>
+      <c r="C12" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="89" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="82">
+        <v>8</v>
+      </c>
+      <c r="D14" s="90">
+        <v>1200</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="77"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="89"/>
+      <c r="G15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1200</v>
+      </c>
+      <c r="M15" s="66" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="80"/>
+      <c r="D16" s="91"/>
+      <c r="G16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="82">
+        <v>2</v>
+      </c>
+      <c r="D17" s="90">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="77"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="89"/>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="83" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="80"/>
+      <c r="D19" s="91"/>
+      <c r="G19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="82">
+        <v>2</v>
+      </c>
+      <c r="D20" s="90">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="77"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="89"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="84" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="80"/>
+      <c r="D22" s="91"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="78">
+        <v>2</v>
+      </c>
+      <c r="D23" s="89">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="82">
+        <v>4</v>
+      </c>
+      <c r="D24" s="90">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="77"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="89"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="80"/>
+      <c r="D26" s="91"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="78">
+        <v>1</v>
+      </c>
+      <c r="D27" s="89">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="82">
+        <v>2</v>
+      </c>
+      <c r="D28" s="90">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="77"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="89"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="80"/>
+      <c r="D30" s="91"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="82">
+        <v>2</v>
+      </c>
+      <c r="D31" s="90">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="77"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="89"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="79" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="80"/>
+      <c r="D33" s="91"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="78">
+        <v>1</v>
+      </c>
+      <c r="D34" s="89">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="82">
+        <v>2</v>
+      </c>
+      <c r="D35" s="90">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="77"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="89"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="79" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="80"/>
+      <c r="D37" s="91"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="82">
+        <v>4</v>
+      </c>
+      <c r="D38" s="90">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="77"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="89"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="87" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="88"/>
+      <c r="D40" s="91"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="78">
+        <v>12</v>
+      </c>
+      <c r="D41" s="89">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="82">
+        <v>5</v>
+      </c>
+      <c r="D42" s="90">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="92" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="92"/>
+      <c r="D44" s="93">
+        <v>1550000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M15:O15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>